<commit_message>
edit to data description
</commit_message>
<xml_diff>
--- a/Data/London_SES_data.xlsx
+++ b/Data/London_SES_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Schroeder-et-al.--2023----An-extended-period-of-elevated-influenza-mortality-risk-follows-the-main-waves-of-influenza-pandemics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7863EFD2-F512-42FC-AC9F-7540D2346E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E87D5AE-19D3-4789-8864-B24B13387E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{79163AD3-1606-4ECB-BAC9-2F1C9457D574}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{79163AD3-1606-4ECB-BAC9-2F1C9457D574}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="3" r:id="rId1"/>
@@ -151,16 +151,19 @@
     <t>proportion of people living in small tenements with more than 2 occupants per room to the population</t>
   </si>
   <si>
-    <t>(Derived) OC_pesmteoc divided by pop_census</t>
-  </si>
-  <si>
     <t>Borough</t>
   </si>
   <si>
-    <t>This file contains information on infant mortality and measure of overcrowding for the Boroughs of London, averaged over the years 1900 - 1917, as collected from the Medical Officer for Health Reports and other sources. For more details, see the description in Section A.5 of the Supplementary Information accompanying the main article. We are grateful to Siqi Qiao for providing us with the data. Used with permission.</t>
-  </si>
-  <si>
     <t>This Excel file contains the data for the additional analysis for London used in this study.</t>
+  </si>
+  <si>
+    <t>This file contains information on infant mortality and measure of overcrowding for the Boroughs of London, averaged over the years 1900 - 1917, as collected from the Medical Officer for Health Reports, MOH reports (1901), the census report (1911) and the “The New Survey” (1921). For more details, see the description in Section A.5 of the Supplementary Information accompanying the main article. We are grateful to Siqi Qiao for providing us with the data. Used with permission.</t>
+  </si>
+  <si>
+    <t>Derived measure based on: 1. 1891 (sheet 1, sanitary area): 1892 MOH Report, P4-7; 1891 (sheet 2, Met. B.): The New Survey Vol I, P162-163
+2. 1901: 1901 MOH Report, P2-6
+3. 1911: 1911 Census, Report 12 , Pxviii
+4. 1921: The New Survey Vol I, P162-163</t>
   </si>
 </sst>
 </file>
@@ -571,7 +574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2A0E65-518C-4D86-A83E-AB3102A8EC9C}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -580,10 +585,10 @@
   <sheetData>
     <row r="1" spans="1:1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -597,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F197C40B-C3FC-432B-BC0F-C00533FBC835}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -638,7 +643,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -672,7 +677,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>29</v>

</xml_diff>